<commit_message>
Products Excel File Changed
</commit_message>
<xml_diff>
--- a/src/assets/samples/SampleProducts.xlsx
+++ b/src/assets/samples/SampleProducts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">ParentProductCode</t>
   </si>
@@ -70,9 +70,6 @@
     <t xml:space="preserve">Currency</t>
   </si>
   <si>
-    <t xml:space="preserve">CurrencyId</t>
-  </si>
-  <si>
     <t xml:space="preserve">NetPrice</t>
   </si>
   <si>
@@ -83,15 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ManufacturerPartNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gtin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
   </si>
 </sst>
 </file>
@@ -276,13 +264,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1048576"/>
+  <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="14.43"/>
@@ -351,19 +339,10 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
@@ -390,7 +369,6 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>